<commit_message>
- Implemented a new Python script `visualize_ruleflow.py` for hierarchical visualization of the ruleflow in the Delphes decision engine, including package and rule extraction, execution order analysis, and Mermaid diagram generation. - Created `check_known_issues_sync.py` to validate the "Known Issues" section in the README against GitHub issues, ensuring all listed issues are open and correctly linked. - Added unit tests for `LocalizedApp.handle_case` to validate required fields and distribution engine handling.
</commit_message>
<xml_diff>
--- a/tests/Emails type.xlsx
+++ b/tests/Emails type.xlsx
@@ -5,22 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E748F71-C6B2-8C47-AC0D-10F28E21F48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E518F4F-AD39-D544-A0AD-A78C78780C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuille1!$A$1:$I$65</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="439">
   <si>
     <t>AGDREF</t>
   </si>
@@ -41,22 +57,6 @@
   </si>
   <si>
     <t>Texte Mail</t>
-  </si>
-  <si>
-    <t>28/12/2025 22:43:19
-mistral-small-3.1-24b-instruct-2503</t>
-  </si>
-  <si>
-    <t>29/12/2025 13:23:06
-mistral-small-3.1-24b-instruct-2503</t>
-  </si>
-  <si>
-    <t>29/12/2025 13:58:50
-mistral-small-3.1-24b-instruct-2503</t>
-  </si>
-  <si>
-    <t>29/12/2025 14:01:50
-mistral-small-3.1-24b-instruct-2503</t>
   </si>
   <si>
     <t>0000000001</t>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>Intentions (temps de réponse : 13.34 secondes) :
+1/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 11.49 secondes) :
+1/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 2.83 secondes) :
 1/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -103,6 +115,15 @@
 1/ DEPOT DE DEMANDE D'ASILE
    - Score: 9
    - Justification: Le demandeur exprime clairement qu'il souhaite déposer une demande de droit d'asile.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 1.12 secondes) :
+1/ DEPOT DE DEMANDE D'ASILE
+   - Score: 10
+   - Justification: Le texte mentionne explicitement une demande d'asile.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -136,6 +157,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 4.52 secondes) :
+1/ EXPIRATION D'UNE API
+   - Score: 10
+   - Justification: Le texte mentionne explicitement l'expiration de l'attestation de prolongation d'instruction (API) depuis le 11 octobre 2024.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000004</t>
   </si>
   <si>
@@ -155,10 +185,10 @@
     <t>ERREUR: HTTP 500 - Internal Server Error</t>
   </si>
   <si>
-    <t>Intentions (temps de réponse : 7.15 secondes) :
+    <t>Intentions (temps de réponse : 11.89 secondes) :
 1/ EXPIRATION D'UNE API
    - Score: 10
-   - Justification: Le texte mentionne explicitement l'expiration de l'API de Mme D et demande son renouvellement.
+   - Justification: Le texte mentionne explicitement l'expiration de l'API de Mme D.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -190,6 +220,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 3.65 secondes) :
+1/ EXPIRATION D'UNE API
+   - Score: 10
+   - Justification: Le texte mentionne explicitement l'expiration de l'API de Mr E E.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000006</t>
   </si>
   <si>
@@ -207,6 +246,15 @@
   </si>
   <si>
     <t>Intentions (temps de réponse : 1.38 secondes) :
+1/ OU EN EST MA DEMANDE D'ASILE EN COURS
+   - Score: 10
+   - Justification: Le demandeur souhaite savoir où sa demande d'asile en est.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 2.85 secondes) :
 1/ OU EN EST MA DEMANDE D'ASILE EN COURS
    - Score: 10
    - Justification: Le demandeur souhaite savoir où sa demande d'asile en est.
@@ -235,6 +283,15 @@
 1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
    - Score: 10
    - Justification: Le texte mentionne explicitement une demande de renouvellement de récépissé.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 12.63 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
+   - Score: 10
+   - Justification: Le demandeur sollicite la prise d'un rendez-vous pour le renouvellement de son récépissé. Cette intention ne vaut que pour un récépissé. Ni pour un titre de séjour, ni pour une ATDA.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -276,6 +333,18 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 11.58 secondes) :
+1/ EXPIRATION D'UNE ATDA
+   - Score: 10
+   - Justification: Le texte mentionne explicitement l'expiration de l'ATDA le 23/11/2024.
+2/ MISE A JOUR INFOS ATDA
+   - Score: 10
+   - Justification: Le texte mentionne une demande de rendez-vous pour le renouvellement de l'ATDA, ce qui implique une mise à jour des informations.
+3/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000009</t>
   </si>
   <si>
@@ -296,6 +365,12 @@
   </si>
   <si>
     <t>Intentions (temps de réponse : 12.16 secondes) :
+1/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 11.51 secondes) :
 1/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -329,6 +404,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 4.76 secondes) :
+1/ DIFFICULTES AVEC LE SITE DE L'ANEF
+   - Score: 8
+   - Justification: Le demandeur mentionne explicitement qu'il n'arrive pas à demander un titre de voyage sur ANEF.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000011</t>
   </si>
   <si>
@@ -360,6 +444,18 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 3.81 secondes) :
+1/ EXPIRATION D'UNE ATDA
+   - Score: 8
+   - Justification: Le demandeur mentionne explicitement qu'il souhaite renouveler son ATDA car son nouveau rendez-vous est le 10/12/2024, ce qui implique que son ATDA actuel va expirer.
+2/ MISE A JOUR INFOS ATDA
+   - Score: 3
+   - Justification: Le demandeur mentionne son nouveau numéro de téléphone, mais ne fournit pas d'autres informations nouvelles concernant son ATDA.
+3/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000012</t>
   </si>
   <si>
@@ -385,6 +481,15 @@
 1/ EXPIRATION D'UNE ATDA
    - Score: 10
    - Justification: Le texte mentionne explicitement l'expiration de l'ATDA de Mme L L, qui a expiré le 19/09/2024.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 12.36 secondes) :
+1/ EXPIRATION D'UNE ATDA
+   - Score: 10
+   - Justification: Le texte mentionne explicitement l'expiration de l'ATDA de Mme L L.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -420,6 +525,21 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 4.32 secondes) :
+1/ EXPIRATION D'UNE API
+   - Score: 10
+   - Justification: Le texte mentionne explicitement l'expiration d'une API.
+2/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 10
+   - Justification: Le texte mentionne la nécessité de prendre un rendez-vous pour une demande de titre de séjour, mais ne mentionne pas l'ANEF.
+3/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 10
+   - Justification: Le texte mentionne explicitement des difficultés à obtenir un rendez-vous.
+4/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000014</t>
   </si>
   <si>
@@ -443,6 +563,18 @@
    - Score: 10
    - Justification: Le texte mentionne explicitement la nécessité de faire des démarches pour des papiers, ce qui peut correspondre à une première demande de titre de séjour.
 4/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 4.52 secondes) :
+1/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 10
+   - Justification: Le demandeur exprime explicitement une difficulté à prendre un rendez-vous et demande un rendez-vous directement à la préfecture.
+2/ DIFFICULTES AVEC LE SITE DE L'ANEF
+   - Score: 8
+   - Justification: Le demandeur mentionne qu'il a des difficultés avec le site de l'ANEF et qu'il n'est pas reconnu en tant que tel.
+3/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -468,6 +600,30 @@
    - Score: 10
    - Justification: Le texte mentionne explicitement une demande de rendez-vous pour Monsieur O O.
 2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 3.73 secondes) :
+1/ DIFFICULTES AVEC LE SITE DE L'ANEF
+   - Score: 4
+   - Justification: Le texte mentionne un problème avec l'ANEF, mais il n'est pas clair si cela concerne la navigation sur le site ou un autre aspect.
+2/ PRISE DE RENDEZ-VOUS REMISE DE TITRES
+   - Score: 3
+   - Justification: Le texte demande un rendez-vous, mais il n'est pas spécifié si c'est pour la remise d'un titre.
+3/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
+   - Score: 3
+   - Justification: Le texte demande un rendez-vous, mais il n'est pas spécifié si c'est pour le renouvellement d'un récépissé.
+4/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 3
+   - Justification: Le texte demande un rendez-vous, mais il n'est pas spécifié si c'est pour le renouvellement d'un titre de séjour en dehors de l'ANEF.
+5/ PRISE DE RENDEZ-VOUS SAUF-CONDUITS
+   - Score: 3
+   - Justification: Le texte demande un rendez-vous, mais il n'est pas spécifié si c'est pour un sauf-conduit.
+6/ PRISE DE RENDEZ-VOUS PREMIERE DEMANDE DE TITRE DE SEJOUR
+   - Score: 3
+   - Justification: Le texte demande un rendez-vous, mais il n'est pas spécifié si c'est pour une première demande de titre de séjour.
+7/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -504,6 +660,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 3.46 secondes) :
+1/ PRISE DE RENDEZ-VOUS REMISE DE TITRES
+   - Score: 10
+   - Justification: Le demandeur souhaite prendre un rendez-vous pour la remise d'un titre de voyage. Le texte mentionne explicitement la demande de rendez-vous pour résoudre un problème lié à la demande de titre de voyage.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000017</t>
   </si>
   <si>
@@ -525,6 +690,12 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 2.74 secondes) :
+1/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000018</t>
   </si>
   <si>
@@ -541,6 +712,15 @@
 1/ DEMANDE EN RAPPORT AVEC PROCEDURE DUBLIN EN COURS
    - Score: 10
    - Justification: Le demandeur mentionne explicitement qu'il a été détenu à l'aéroport en raison d'une procédure Dublin impliquant Malte.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 1.70 secondes) :
+1/ DEMANDE EN RAPPORT AVEC PROCEDURE DUBLIN EN COURS
+   - Score: 10
+   - Justification: Le demandeur mentionne explicitement qu'il a initié sa demande dans un autre pays de l'Union Européenne (Malte) que la France, ce qui indique une procédure Dublin en cours.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -570,6 +750,12 @@
    - Score: 10
    - Justification: Le texte mentionne explicitement la demande de génération d'un DCEM, ce qui correspond à une demande de duplicata.
 2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 11.56 secondes) :
+1/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -604,6 +790,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 12.37 secondes) :
+1/ DEMANDE EN RAPPORT AVEC PROCEDURE DUBLIN EN COURS
+   - Score: 10
+   - Justification: Le texte mentionne explicitement une procédure Dublin en cours et demande sa clôture.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000021</t>
   </si>
   <si>
@@ -629,6 +824,84 @@
    - Score: 10
    - Justification: Le demandeur mentionne qu'il a déjà 10 permis de séjour et qu'il n'a pas pu en prendre un nouveau, ce qui implique qu'il cherche à renouveler son titre de séjour.
 3/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 11.31 secondes) :
+1/ PRISE DE RENDEZ-VOUS REMISE DE TITRES
+   - Score: 10
+   - Justification: Le demandeur exprime clairement qu'il attend depuis 15 mois et demande un titre de séjour.
+2/ PRISE DE RENDEZ-VOUS PREMIERE DEMANDE DE TITRE DE SEJOUR
+   - Score: 10
+   - Justification: Le demandeur exprime clairement qu'il attend depuis 15 mois et demande un titre de séjour pour la première fois.
+3/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 1
+   - Justification: Le texte ne mentionne aucune difficulté à prendre un rendez-vous.
+4/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de renouvellement de récépissé.
+5/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de renouvellement de titre de séjour hors ANEF.
+6/ PRISE DE RENDEZ-VOUS SAUF-CONDUITS
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de sauf-conduit.
+7/ DEMANDE D'UN ETUDIANT EN PROGRAMME DE MOBILITE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande en lien avec un programme de mobilité étudiante.
+8/ DEMANDE D'UN STAGIAIRE ASSOCIE EN PROFESSION MEDICALE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande en lien avec un stage en profession médicale.
+9/ CHANGEMENT STATUT ETUDIANT A SALARIE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de changement de statut d'étudiant à salarié.
+10/ CHANGEMENT STATUT ETUDIANT A RECHERCHE D'EMPLOI
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de changement de statut d'étudiant à demandeur d'emploi.
+11/ JE VEUX RETOURNER DANS MON PAYS POUR MOTIF EXCEPTIONNEL
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de retour dans le pays d'origine pour motif exceptionnel.
+12/ DIFFICULTES AVEC LE SITE DE L'ANEF
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de difficulté avec le site de l'ANEF.
+13/ DEMANDE EN RAPPORT AVEC PROCEDURE DUBLIN EN COURS
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande en rapport avec une procédure Dublin en cours.
+14/ DEPOT DE DEMANDE D'ASILE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande d'asile.
+15/ OU EN EST MA DEMANDE D'ASILE EN COURS
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande d'asile en cours.
+16/ RESSORTISSANT UKRAINIEN DEMANDE UN NOUVEAU TITRE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas la nationalité ukrainienne du demandeur.
+17/ RESSORTISSANT UKRAINIEN DEMANDE RENOUVELLEMENT DE SON TITRE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas la nationalité ukrainienne du demandeur.
+18/ RESSORTISSANT UKRAINIEN AUTRE DEMANDE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas la nationalité ukrainienne du demandeur.
+19/ EXPIRATION D'UNE API
+   - Score: 1
+   - Justification: Le texte ne mentionne pas d'expiration d'une API.
+20/ EXPIRATION D'UNE ATDA
+   - Score: 1
+   - Justification: Le texte ne mentionne pas d'expiration d'une ATDA.
+21/ MISE A JOUR INFOS ATDA
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de mise à jour d'informations concernant une ATDA.
+22/ DEMANDE D'HEBERGEMENT D'URGENCE POUR UN DEMANDEUR D'ASILE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande d'hébergement d'urgence.
+23/ DEMANDE D'AIDE FINANCIERE POUR UN DEMANDEUR D'ASILE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande d'aide financière.
+24/ DEMANDE DE DUPLICATA
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de duplicata.
+25/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -662,6 +935,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 3.35 secondes) :
+1/ PRISE DE RENDEZ-VOUS PREMIERE DEMANDE DE TITRE DE SEJOUR
+   - Score: 10
+   - Justification: Le demandeur mentionne explicitement qu'il s'agit de sa première demande de carte de séjour.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000023</t>
   </si>
   <si>
@@ -685,6 +967,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 2.96 secondes) :
+1/ PRISE DE RENDEZ-VOUS PREMIERE DEMANDE DE TITRE DE SEJOUR
+   - Score: 10
+   - Justification: Le demandeur souhaite prendre un rendez-vous pour une première demande de titre de séjour.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000024</t>
   </si>
   <si>
@@ -704,6 +995,15 @@
 1/ JE VEUX RETOURNER DANS MON PAYS POUR MOTIF EXCEPTIONNEL
    - Score: 10
    - Justification: Le demandeur souhaite retourner dans son pays pour des raisons exceptionnelles (maladie de son père).
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 3.03 secondes) :
+1/ JE VEUX RETOURNER DANS MON PAYS POUR MOTIF EXCEPTIONNEL
+   - Score: 10
+   - Justification: Le demandeur mentionne explicitement qu'il doit retourner dans son pays en raison de la maladie de son père, ce qui constitue un motif exceptionnel.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -752,6 +1052,18 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 3.35 secondes) :
+1/ EXPIRATION D'UNE ATDA
+   - Score: 10
+   - Justification: Le texte mentionne explicitement la demande de renouvellement de l'ATDA.
+2/ MISE A JOUR INFOS ATDA
+   - Score: 10
+   - Justification: Le texte mentionne explicitement la demande de renouvellement de l'ATDA avec la nouvelle adresse.
+3/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000026</t>
   </si>
   <si>
@@ -782,6 +1094,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 2.57 secondes) :
+1/ DEMANDE EN RAPPORT AVEC PROCEDURE DUBLIN EN COURS
+   - Score: 10
+   - Justification: Le demandeur fait explicitement mention d'un transfert de dossier vers l'Allemagne dans le cadre d'une procédure Dublin.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000027</t>
   </si>
   <si>
@@ -807,6 +1128,12 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 2.92 secondes) :
+1/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000028</t>
   </si>
   <si>
@@ -824,6 +1151,15 @@
    - Score: 10
    - Justification: Le demandeur mentionne son numéro d'asile et demande de l'aide, ce qui implique qu'il souhaite savoir où en est sa demande d'asile.
 3/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 2.69 secondes) :
+1/ DEMANDE EN RAPPORT AVEC PROCEDURE DUBLIN EN COURS
+   - Score: 10
+   - Justification: Le demandeur mentionne explicitement qu'il était en procédure Dublin en 2017.
+2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -866,6 +1202,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 3.42 secondes) :
+1/ DEMANDE EN RAPPORT AVEC PROCEDURE DUBLIN EN COURS
+   - Score: 10
+   - Justification: Le texte mentionne explicitement une demande d'informations en rapport avec une procédure Dublin en cours.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000030</t>
   </si>
   <si>
@@ -895,6 +1240,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 3.40 secondes) :
+1/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 8
+   - Justification: Le demandeur exprime une difficulté à prendre un rendez-vous pour éclaircir une situation administrative.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000031</t>
   </si>
   <si>
@@ -911,6 +1265,15 @@
 1/ EXPIRATION D'UNE API
    - Score: 10
    - Justification: Le texte mentionne explicitement une API, ce qui est un document provisoire lié à une demande de titre de séjour.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 0.95 secondes) :
+1/ EXPIRATION D'UNE API
+   - Score: 10
+   - Justification: Le texte mentionne explicitement l'API, ce qui indique que le document provisoire a expiré ou est sur le point d'expirer.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -956,6 +1319,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 12.31 secondes) :
+1/ DIFFICULTES AVEC LE SITE DE L'ANEF
+   - Score: 10
+   - Justification: Le demandeur mentionne explicitement qu'il rencontre des difficultés à modifier son adresse sur le site de l'ANEF.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000033</t>
   </si>
   <si>
@@ -987,6 +1359,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 4.15 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
+   - Score: 10
+   - Justification: Le demandeur souhaite obtenir un récépissé en attendant la délivrance de son nouveau titre de séjour.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000034</t>
   </si>
   <si>
@@ -1015,6 +1396,18 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 12.46 secondes) :
+1/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 10
+   - Justification: Le texte mentionne explicitement des difficultés à prendre un rendez-vous.
+2/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 10
+   - Justification: Le texte mentionne une demande de rendez-vous pour le renouvellement d'un titre de séjour, et il est fait référence à des difficultés sur le site de la préfecture, ce qui indique un processus en dehors de l'ANEF.
+3/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000035</t>
   </si>
   <si>
@@ -1037,6 +1430,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 2.61 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 10
+   - Justification: Le demandeur souhaite prendre un rendez-vous pour le renouvellement de son titre de séjour.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000036</t>
   </si>
   <si>
@@ -1061,6 +1463,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 2.55 secondes) :
+1/ PRISE DE RENDEZ-VOUS REMISE DE TITRES
+   - Score: 10
+   - Justification: Le demandeur souhaite savoir si sa carte est disponible, ce qui correspond à la remise de titre.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000037</t>
   </si>
   <si>
@@ -1081,6 +1492,90 @@
    - Score: 10
    - Justification: Le texte mentionne explicitement la nécessité d'une carte de résidente pour des démarches, ce qui suggère une demande de duplicata.
 2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 12.01 secondes) :
+1/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 12.21 secondes) :
+1/ DEMANDE DE DUPLICATA
+   - Score: 10
+   - Justification: Le texte mentionne la nécessité d'une carte de résidente pour des démarches, ce qui peut impliquer une demande de duplicata.
+2/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de difficulté à prendre un rendez-vous.
+3/ PRISE DE RENDEZ-VOUS REMISE DE TITRES
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de rendez-vous pour la remise d'un titre.
+4/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de rendez-vous pour le renouvellement d'un récépissé.
+5/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de rendez-vous pour le renouvellement d'un titre de séjour en dehors de l'ANEF.
+6/ PRISE DE RENDEZ-VOUS SAUF-CONDUITS
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de rendez-vous pour un sauf-conduit.
+7/ PRISE DE RENDEZ-VOUS PREMIERE DEMANDE DE TITRE DE SEJOUR
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de rendez-vous pour une première demande de titre de séjour.
+8/ EXPIRATION D'UNE API
+   - Score: 1
+   - Justification: Le texte ne mentionne pas l'expiration d'une API.
+9/ DEPOT DE DEMANDE D'ASILE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de dépôt d'asile.
+10/ OU EN EST MA DEMANDE D'ASILE EN COURS
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande d'information sur une demande d'asile en cours.
+11/ EXPIRATION D'UNE ATDA
+   - Score: 1
+   - Justification: Le texte ne mentionne pas l'expiration d'une ATDA.
+12/ MISE A JOUR INFOS ATDA
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de mise à jour d'informations concernant une ATDA.
+13/ DEMANDE EN RAPPORT AVEC PROCEDURE DUBLIN EN COURS
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande en rapport avec une procédure Dublin en cours.
+14/ RESSORTISSANT UKRAINIEN DEMANDE UN NOUVEAU TITRE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande d'un nouveau titre de séjour pour un ressortissant ukrainien.
+15/ RESSORTISSANT UKRAINIEN DEMANDE RENOUVELLEMENT DE SON TITRE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de renouvellement de titre de séjour pour un ressortissant ukrainien.
+16/ RESSORTISSANT UKRAINIEN AUTRE DEMANDE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas d'autre demande pour un ressortissant ukrainien.
+17/ DEMANDE D'UN ETUDIANT EN PROGRAMME DE MOBILITE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande d'étudiant en programme de mobilité.
+18/ DEMANDE D'UN STAGIAIRE ASSOCIE EN PROFESSION MEDICALE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de stagiaire associé en profession médicale.
+19/ DIFFICULTES AVEC LE SITE DE L'ANEF
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de difficultés avec le site de l'ANEF.
+20/ CHANGEMENT STATUT ETUDIANT A SALARIE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de changement de statut d'étudiant à salarié.
+21/ CHANGEMENT STATUT ETUDIANT A RECHERCHE D'EMPLOI
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de changement de statut d'étudiant à demandeur d'emploi.
+22/ JE VEUX RETOURNER DANS MON PAYS POUR MOTIF EXCEPTIONNEL
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande de retour dans le pays pour motif exceptionnel.
+23/ DEMANDE D'HEBERGEMENT D'URGENCE POUR UN DEMANDEUR D'ASILE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande d'hébergement d'urgence pour un demandeur d'asile.
+24/ DEMANDE D'AIDE FINANCIERE POUR UN DEMANDEUR D'ASILE
+   - Score: 1
+   - Justification: Le texte ne mentionne pas de demande d'aide financière pour un demandeur d'asile.
+25/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -1113,6 +1608,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 12.92 secondes) :
+1/ CHANGEMENT STATUT ETUDIANT A SALARIE
+   - Score: 10
+   - Justification: Le demandeur souhaite déclarer un changement de statut d'étudiant à salarié.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000039</t>
   </si>
   <si>
@@ -1138,6 +1642,12 @@
    - Score: 10
    - Justification: Le texte mentionne explicitement un rendez-vous pour le dépôt de demande de titre de séjour.
 2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 11.32 secondes) :
+1/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -1181,6 +1691,18 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 4.71 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 10
+   - Justification: Le demandeur exprime clairement sa difficulté à prendre un rendez-vous pour le renouvellement de son titre de séjour, et mentionne explicitement qu'il a essayé de se connecter via l'ANEF sans succès.
+2/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 10
+   - Justification: Le demandeur décrit en détail les multiples tentatives infructueuses pour prendre un rendez-vous, y compris par téléphone, par mail, et via l'ANEF.
+3/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000041</t>
   </si>
   <si>
@@ -1203,6 +1725,15 @@
 1/ DIFFICULTES AVEC LE SITE DE L'ANEF
    - Score: 8
    - Justification: Le demandeur mentionne explicitement qu'il n'arrive pas à faire sa demande de passeport talent sur le site de l'ANEF.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 2.51 secondes) :
+1/ DIFFICULTES AVEC LE SITE DE L'ANEF
+   - Score: 10
+   - Justification: Le texte mentionne explicitement que l'usager a des difficultés à naviguer sur le site de l'ANEF.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -1264,6 +1795,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 11.80 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 10
+   - Justification: Le demandeur souhaite prendre un rendez-vous pour le renouvellement de son titre de séjour et sa demande s'inscrit dans un processus géré en dehors du site de l'ANEF.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000044</t>
   </si>
   <si>
@@ -1290,6 +1830,15 @@
    - Score: 10
    - Justification: Le demandeur demande explicitement où en est le statut de son dossier de renouvellement de titre de séjour.
 3/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 11.70 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
+   - Score: 10
+   - Justification: Le texte mentionne explicitement que le récépissé expire bientôt, ce qui implique une demande de renouvellement.
+2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -1327,6 +1876,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 3.76 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 10
+   - Justification: Le demandeur souhaite avancer son rendez-vous pour le renouvellement de son titre de séjour, ce qui correspond à cette intention.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000046</t>
   </si>
   <si>
@@ -1359,6 +1917,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 4.34 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
+   - Score: 10
+   - Justification: Le demandeur sollicite la prise d'un rendez-vous pour le renouvellement de son récépissé.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000047</t>
   </si>
   <si>
@@ -1381,6 +1948,12 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 11.62 secondes) :
+1/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000048</t>
   </si>
   <si>
@@ -1400,6 +1973,15 @@
 1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
    - Score: 10
    - Justification: Le demandeur souhaite prendre un rendez-vous pour le renouvellement de son titre de séjour. Sa demande s'inscrit dans un processus géré en dehors du site de l'ANEF.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 11.54 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 9
+   - Justification: Le demandeur souhaite prendre un rendez-vous pour le renouvellement de son titre de séjour.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -1424,6 +2006,15 @@
 1/ CHANGEMENT STATUT ETUDIANT A SALARIE
    - Score: 10
    - Justification: Le demandeur souhaite déclarer un changement de statut d'étudiant à salarié.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 2.48 secondes) :
+1/ CHANGEMENT STATUT ETUDIANT A SALARIE
+   - Score: 10
+   - Justification: Le demandeur exprime clairement sa volonté de changer son statut d'étudiant à salarié.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -1459,6 +2050,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 12.43 secondes) :
+1/ CHANGEMENT STATUT ETUDIANT A SALARIE
+   - Score: 10
+   - Justification: Le texte mentionne explicitement une demande de changement de statut d'étudiant à salarié.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000051</t>
   </si>
   <si>
@@ -1478,6 +2078,18 @@
    - Score: 10
    - Justification: Le demandeur mentionne explicitement que sa carte provisoire a expiré le 27/09/2024, ce qui correspond à l'expiration d'une API.
 2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 12.44 secondes) :
+1/ EXPIRATION D'UNE API
+   - Score: 10
+   - Justification: Le texte mentionne explicitement l'expiration de la carte provisoire, qui est une API.
+2/ DEMANDE D'AIDE FINANCIERE POUR UN DEMANDEUR D'ASILE
+   - Score: 10
+   - Justification: Le texte mentionne explicitement une incapacité financière et une demande d'aide.
+3/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -1504,6 +2116,18 @@
    - Score: 8
    - Justification: Le texte mentionne une difficulté à prendre un rendez-vous dans les prochains jours.
 2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 11.87 secondes) :
+1/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 10
+   - Justification: Le texte mentionne explicitement une difficulté à prendre un rendez-vous.
+2/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
+   - Score: 10
+   - Justification: Le texte mentionne une demande de renouvellement de titre de séjour et indique des difficultés à prendre un rendez-vous.
+3/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -1529,12 +2153,6 @@
 Merci par avance pour votre retour </t>
   </si>
   <si>
-    <t>Intentions (temps de réponse : 14.19 secondes) :
-1/ AUTRE
-   - Score: 1
-   - Justification: Fallback</t>
-  </si>
-  <si>
     <t>0000000054</t>
   </si>
   <si>
@@ -1564,6 +2182,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 11.28 secondes) :
+1/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 8
+   - Justification: Le texte mentionne une difficulté à obtenir un rendez-vous pour récupérer le titre de voyage du fils, ce qui est lié à la prise de rendez-vous.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000055</t>
   </si>
   <si>
@@ -1592,6 +2219,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 2.44 secondes) :
+1/ DEMANDE DE DUPLICATA
+   - Score: 10
+   - Justification: Le demandeur mentionne explicitement qu'il souhaite obtenir un duplicata de sa carte de séjour volée.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000056</t>
   </si>
   <si>
@@ -1614,6 +2250,15 @@
 1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF
    - Score: 8
    - Justification: Le demandeur souhaite envoyer son dossier par voie postale pour le renouvellement de son titre de séjour, ce qui correspond à une demande de renouvellement en dehors du site de l'ANEF.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 11.88 secondes) :
+1/ EXPIRATION D'UNE API
+   - Score: 5
+   - Justification: L'usager mentionne que le délai d'expiration est court, mais ne mentionne pas explicitement l'API.
 2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -1646,6 +2291,12 @@
    - Score: 10
    - Justification: Le demandeur sollicite des informations sur l'avancement de son dossier de renouvellement de titre de séjour, ce qui correspond à une demande de rendez-vous pour le renouvellement d'un titre de séjour en dehors du site de l'ANEF.
 2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 12.39 secondes) :
+1/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -1685,6 +2336,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 13.37 secondes) :
+1/ EXPIRATION D'UNE API
+   - Score: 10
+   - Justification: Le demandeur mentionne explicitement que son titre de séjour expire aujourd'hui et qu'il n'a pas encore reçu l'attestation de prolongation d'instruction.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000059</t>
   </si>
   <si>
@@ -1717,6 +2377,15 @@
    - Score: 5
    - Justification: Le demandeur mentionne avoir reçu plusieurs récépissés, mais ne demande pas explicitement un rendez-vous pour le renouvellement du récépissé.
 4/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>Intentions (temps de réponse : 3.04 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
+   - Score: 10
+   - Justification: Le demandeur sollicite la prise d'un rendez-vous pour le renouvellement de son récépissé.
+2/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
   </si>
@@ -1752,6 +2421,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 2.55 secondes) :
+1/ CHANGEMENT STATUT ETUDIANT A SALARIE
+   - Score: 10
+   - Justification: Le demandeur exprime clairement sa volonté de changer de statut d'étudiant à salarié.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000061</t>
   </si>
   <si>
@@ -1782,6 +2460,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 1.18 secondes) :
+1/ PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE
+   - Score: 10
+   - Justification: Le texte mentionne explicitement le renouvellement d'un récépissé et la demande de prise de rendez-vous.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000062</t>
   </si>
   <si>
@@ -1797,13 +2484,13 @@
 BJ</t>
   </si>
   <si>
-    <t>Intentions (temps de réponse : 3.80 secondes) :
+    <t>Intentions (temps de réponse : 3.45 secondes) :
 1/ PRISE DE RENDEZ-VOUS REMISE DE TITRES
    - Score: 10
-   - Justification: Le demandeur souhaite prendre un rendez-vous pour récupérer sa carte de séjour qui est déjà prête.
+   - Justification: Le demandeur exprime clairement qu'il souhaite prendre un rendez-vous pour récupérer sa carte de séjour, indiquant que celle-ci est déjà prête.
 2/ DIFFICULTES AVEC LE SITE DE L'ANEF
    - Score: 5
-   - Justification: Le demandeur mentionne des difficultés à trouver un rendez-vous sur le lien fourni, ce qui pourrait indiquer un problème avec le site de l'ANEF.
+   - Justification: Le demandeur mentionne qu'il n'arrive pas à trouver un rendez-vous sur le lien fourni, ce qui pourrait indiquer une difficulté avec le site de l'ANEF, mais cela n'est pas explicitement confirmé.
 3/ AUTRE
    - Score: 1
    - Justification: Fallback</t>
@@ -1841,6 +2528,15 @@
    - Justification: Fallback</t>
   </si>
   <si>
+    <t>Intentions (temps de réponse : 11.44 secondes) :
+1/ DIFFICULTE DE PRISE DE RENDEZ-VOUS
+   - Score: 10
+   - Justification: Le texte mentionne explicitement une difficulté à trouver un rendez-vous.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
     <t>0000000064</t>
   </si>
   <si>
@@ -1868,12 +2564,34 @@
    - Score: 1
    - Justification: Fallback</t>
   </si>
+  <si>
+    <t>Intentions (temps de réponse : 2.38 secondes) :
+1/ PRISE DE RENDEZ-VOUS REMISE DE TITRES
+   - Score: 10
+   - Justification: Le texte mentionne explicitement la remise de titre.
+2/ AUTRE
+   - Score: 1
+   - Justification: Fallback</t>
+  </si>
+  <si>
+    <t>53 ok
+9  à améliorer
+2 ko</t>
+  </si>
+  <si>
+    <t>28/12/2025 15:43:19
+mistral-small-3.1-24b-instruct-2503</t>
+  </si>
+  <si>
+    <t>05/01/2026 10:54:49
+mistral-small-3.1-24b-instruct-2503</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1963,13 +2681,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1982,33 +2693,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -2101,27 +2785,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2206,7 +2875,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="13" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2217,38 +2886,41 @@
     <xf numFmtId="4" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -2602,27 +3274,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="50" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4" style="2" customWidth="1"/>
+    <col min="2" max="3" width="2.796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.19921875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="53.796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.59765625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.3984375" style="2" customWidth="1"/>
     <col min="7" max="7" width="70" style="2" customWidth="1"/>
-    <col min="8" max="8" width="50" customWidth="1"/>
-    <col min="9" max="11" width="50" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="50" style="2"/>
+    <col min="8" max="9" width="50" customWidth="1"/>
+    <col min="10" max="16384" width="50" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="50" customHeight="1">
+    <row r="1" spans="1:10" ht="84">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2644,98 +3317,105 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="J1" s="12">
+        <f>SUBTOTAL(3,I2:I65)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="84">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="84" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="I2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="126">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="126" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="182">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="182" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="140" customHeight="1">
+    <row r="5" spans="1:10" ht="140">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -2746,10 +3426,10 @@
         <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>32</v>
@@ -2757,14 +3437,14 @@
       <c r="G5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="126" customHeight="1">
+    <row r="6" spans="1:10" ht="126">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -2775,10 +3455,10 @@
         <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>38</v>
@@ -2786,1543 +3466,1723 @@
       <c r="G6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="112" customHeight="1">
+      <c r="I6" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="112">
       <c r="A7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="168" customHeight="1">
+      <c r="H7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="168">
       <c r="A8" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="196" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="196">
       <c r="A9" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="70" customHeight="1">
+        <v>59</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="70">
       <c r="A10" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="210" customHeight="1">
+        <v>66</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="210">
       <c r="A11" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="154" customHeight="1">
+        <v>73</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="224">
       <c r="A12" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="140">
+      <c r="A13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="306">
+      <c r="A14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="293">
+      <c r="A15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="F15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="409.6">
+      <c r="A16" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="140" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="306" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="293" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="140" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="280" customHeight="1">
+        <v>106</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="280">
       <c r="A17" s="3" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="70" customHeight="1">
+        <v>113</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="112">
       <c r="A18" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="154" customHeight="1">
+        <v>120</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="293">
       <c r="A19" s="3" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="126" customHeight="1">
+      <c r="H19" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="126">
       <c r="A20" s="3" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="293">
+      <c r="A21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="409.6">
+      <c r="A22" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="224">
+      <c r="A23" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="140">
+      <c r="A24" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="293" customHeight="1">
-      <c r="A21" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="252" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="224" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H23" s="6" t="s">
+      <c r="F24" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="154">
+      <c r="A25" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="345">
+      <c r="A26" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="182">
+      <c r="A27" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="84">
+      <c r="A28" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="210">
+      <c r="A29" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="140" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="140" customHeight="1">
-      <c r="A25" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="345" customHeight="1">
-      <c r="A26" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="182" customHeight="1">
-      <c r="A27" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="84" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="210" customHeight="1">
-      <c r="A29" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="F29" s="3" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="345" customHeight="1">
+        <v>193</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="345">
       <c r="A30" s="3" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="154" customHeight="1">
+        <v>200</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="154">
       <c r="A31" s="3" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="126" customHeight="1">
+        <v>208</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="126">
       <c r="A32" s="3" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="371" customHeight="1">
+        <v>213</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="371">
       <c r="A33" s="3" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="332" customHeight="1">
+        <v>220</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="332">
       <c r="A34" s="3" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="252" customHeight="1">
+        <v>227</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="252">
       <c r="A35" s="3" t="s">
-        <v>201</v>
+        <v>230</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="168" customHeight="1">
+        <v>234</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="168">
       <c r="A36" s="3" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>208</v>
+        <v>238</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>208</v>
+        <v>238</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>209</v>
+        <v>239</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="126" customHeight="1">
+        <v>241</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="126">
       <c r="A37" s="3" t="s">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="154" customHeight="1">
+        <v>247</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="409.6">
       <c r="A38" s="3" t="s">
-        <v>218</v>
+        <v>250</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>220</v>
+        <v>252</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="252" customHeight="1">
+        <v>254</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="252">
       <c r="A39" s="3" t="s">
-        <v>224</v>
+        <v>258</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>226</v>
+        <v>260</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="154" customHeight="1">
+        <v>262</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="154">
       <c r="A40" s="3" t="s">
-        <v>229</v>
+        <v>264</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>230</v>
+        <v>265</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>230</v>
+        <v>265</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>231</v>
+        <v>266</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="409.6">
+      <c r="A41" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="126">
+      <c r="A42" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="140">
+      <c r="A43" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="238">
+      <c r="A44" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="409.5" customHeight="1">
-      <c r="A41" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="126" customHeight="1">
-      <c r="A42" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="140" customHeight="1">
-      <c r="A43" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="238" customHeight="1">
-      <c r="A44" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="F44" s="3" t="s">
-        <v>255</v>
+        <v>293</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="210" customHeight="1">
+        <v>294</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="210">
       <c r="A45" s="3" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>261</v>
+        <v>300</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="238" customHeight="1">
+        <v>301</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="238">
       <c r="A46" s="3" t="s">
-        <v>264</v>
+        <v>304</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>265</v>
+        <v>305</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>265</v>
+        <v>305</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>267</v>
+        <v>307</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="409.5" customHeight="1">
+        <v>308</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="409.6">
       <c r="A47" s="3" t="s">
-        <v>270</v>
+        <v>311</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>272</v>
+        <v>313</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="70" customHeight="1">
+        <v>315</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="70">
       <c r="A48" s="3" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="168" customHeight="1">
+        <v>322</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="168">
       <c r="A49" s="3" t="s">
-        <v>282</v>
+        <v>325</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>283</v>
+        <v>326</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>283</v>
+        <v>326</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>284</v>
+        <v>327</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>285</v>
+        <v>328</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="112" customHeight="1">
+        <v>329</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="126">
       <c r="A50" s="3" t="s">
-        <v>288</v>
+        <v>332</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>289</v>
+        <v>333</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>289</v>
+        <v>333</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>284</v>
+        <v>327</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>290</v>
+        <v>334</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="168" customHeight="1">
+        <v>335</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="168">
       <c r="A51" s="3" t="s">
-        <v>293</v>
+        <v>338</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>294</v>
+        <v>339</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>294</v>
+        <v>339</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>295</v>
+        <v>340</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>296</v>
+        <v>341</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="140" customHeight="1">
+        <v>342</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="182">
       <c r="A52" s="3" t="s">
-        <v>299</v>
+        <v>345</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>301</v>
+        <v>347</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="140" customHeight="1">
+        <v>348</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="210">
       <c r="A53" s="3" t="s">
-        <v>304</v>
+        <v>351</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>305</v>
+        <v>352</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>305</v>
+        <v>352</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>306</v>
+        <v>353</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>307</v>
+        <v>354</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="140" customHeight="1">
+        <v>355</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="140">
       <c r="A54" s="3" t="s">
-        <v>310</v>
+        <v>358</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>311</v>
+        <v>359</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>311</v>
+        <v>359</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>312</v>
+        <v>360</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>313</v>
+        <v>361</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="H54" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="H54" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J54" s="12" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="196" customHeight="1">
+      <c r="I54" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="196">
       <c r="A55" s="3" t="s">
-        <v>316</v>
+        <v>363</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>317</v>
+        <v>364</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>317</v>
+        <v>364</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>318</v>
+        <v>365</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>319</v>
+        <v>366</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="126" customHeight="1">
+        <v>367</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="126">
       <c r="A56" s="3" t="s">
-        <v>322</v>
+        <v>370</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>323</v>
+        <v>371</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>323</v>
+        <v>371</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>324</v>
+        <v>372</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>325</v>
+        <v>373</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="182" customHeight="1">
+        <v>374</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="182">
       <c r="A57" s="3" t="s">
-        <v>328</v>
+        <v>377</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>329</v>
+        <v>378</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>329</v>
+        <v>378</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>330</v>
+        <v>379</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>331</v>
+        <v>380</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="280" customHeight="1">
+        <v>381</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="280">
       <c r="A58" s="3" t="s">
-        <v>334</v>
+        <v>384</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>335</v>
+        <v>385</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>335</v>
+        <v>385</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>336</v>
+        <v>386</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>337</v>
+        <v>387</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="345" customHeight="1">
+        <v>388</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="345">
       <c r="A59" s="3" t="s">
-        <v>340</v>
+        <v>391</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>341</v>
+        <v>392</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>341</v>
+        <v>392</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>336</v>
+        <v>386</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>342</v>
+        <v>393</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="332" customHeight="1">
+        <v>394</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="332">
       <c r="A60" s="3" t="s">
-        <v>345</v>
+        <v>397</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>346</v>
+        <v>398</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>346</v>
+        <v>398</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>347</v>
+        <v>399</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>348</v>
+        <v>400</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="210" customHeight="1">
+        <v>401</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="210">
       <c r="A61" s="3" t="s">
-        <v>351</v>
+        <v>404</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>352</v>
+        <v>405</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>352</v>
+        <v>405</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>353</v>
+        <v>406</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>354</v>
+        <v>407</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="H61" s="6" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="210" customHeight="1">
+        <v>408</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="210">
       <c r="A62" s="3" t="s">
-        <v>357</v>
+        <v>411</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>358</v>
+        <v>412</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>358</v>
+        <v>412</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>359</v>
+        <v>413</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>360</v>
+        <v>414</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="112" customHeight="1">
+        <v>415</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="I62" s="8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="238">
       <c r="A63" s="3" t="s">
-        <v>363</v>
+        <v>418</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>364</v>
+        <v>419</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>364</v>
+        <v>419</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>365</v>
+        <v>420</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="H63" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="H63" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K63" s="14" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="224" customHeight="1">
+      <c r="I63" s="8" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="224">
       <c r="A64" s="3" t="s">
-        <v>368</v>
+        <v>423</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>369</v>
+        <v>424</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>369</v>
+        <v>424</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>370</v>
+        <v>425</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="112" customHeight="1">
+        <v>426</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="I64" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="112">
       <c r="A65" s="3" t="s">
-        <v>373</v>
+        <v>429</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>374</v>
+        <v>430</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>374</v>
+        <v>430</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>375</v>
+        <v>431</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>376</v>
+        <v>432</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="H65" s="10" t="s">
-        <v>378</v>
+        <v>433</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="42">
+      <c r="I67" s="13" t="s">
+        <v>436</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I65" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>

</xml_diff>

<commit_message>
Fix Makefile, update .env.production.example, update .gitignore to inclure .env.integration
</commit_message>
<xml_diff>
--- a/tests/Emails type.xlsx
+++ b/tests/Emails type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E518F4F-AD39-D544-A0AD-A78C78780C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F896C7D9-D949-8047-9333-291810AEA4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2574,17 +2574,17 @@
    - Justification: Fallback</t>
   </si>
   <si>
-    <t>53 ok
-9  à améliorer
-2 ko</t>
-  </si>
-  <si>
     <t>28/12/2025 15:43:19
 mistral-small-3.1-24b-instruct-2503</t>
   </si>
   <si>
     <t>05/01/2026 10:54:49
 mistral-small-3.1-24b-instruct-2503</t>
+  </si>
+  <si>
+    <t>53 ok
+10  à améliorer
+1 ko</t>
   </si>
 </sst>
 </file>
@@ -2907,9 +2907,6 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2921,6 +2918,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -3277,10 +3277,10 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="50" defaultRowHeight="13"/>
@@ -3317,13 +3317,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>437</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>438</v>
-      </c>
-      <c r="J1" s="12">
+      <c r="J1" s="11">
         <f>SUBTOTAL(3,I2:I65)</f>
         <v>64</v>
       </c>
@@ -4395,7 +4395,7 @@
       <c r="H38" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="I38" s="11" t="s">
+      <c r="I38" s="15" t="s">
         <v>257</v>
       </c>
     </row>
@@ -4598,7 +4598,7 @@
       <c r="H45" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="I45" s="11" t="s">
+      <c r="I45" s="9" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5177,8 +5177,8 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="42">
-      <c r="I67" s="13" t="s">
-        <v>436</v>
+      <c r="I67" s="12" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>